<commit_message>
Update excel checkup file
</commit_message>
<xml_diff>
--- a/day_1/day_1_checkup.xlsx
+++ b/day_1/day_1_checkup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icacorp-my.sharepoint.com/personal/dagnija_strike_rimibaltic_com/Documents/Documents/advent-of-code-2021-main/day_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icacorp-my.sharepoint.com/personal/dagnija_strike_rimibaltic_com/Documents/Documents/advent-of-code-2021/day_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{4B9024C2-1C38-4EC5-99F2-CB7F28352F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7AF040E-E51B-4655-AF02-23978EDCB538}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{4B9024C2-1C38-4EC5-99F2-CB7F28352F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34C5268C-C54A-4EA1-BDA7-ED800BBA8341}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{99774160-3835-449D-9285-2D404A0321BF}"/>
   </bookViews>

</xml_diff>